<commit_message>
adicao de relacionamento entre areas e habilidades
</commit_message>
<xml_diff>
--- a/Base-Nacional-Comum-Curricular/BNCC_Ensino_Medio.xlsx
+++ b/Base-Nacional-Comum-Curricular/BNCC_Ensino_Medio.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f93e8886b6eb1993/Área de Trabalho/DANILLO/Faculdade/TCC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f93e8886b6eb1993/Área de Trabalho/DANILLO/Faculdade/TCC/skillmappr/neo4j/database-init/Base-Nacional-Comum-Curricular/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1" documentId="11_643F254A8A2CADD8CB47A425DB9C9A2516AA4A6C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{04A28BAA-BEBC-40BE-B997-95D32F3E522E}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19425" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="15585" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Competências Gerais" sheetId="1" r:id="rId1"/>
@@ -4726,7 +4726,7 @@
   </sheetPr>
   <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -6074,8 +6074,8 @@
   </sheetPr>
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6420,7 +6420,7 @@
   <dimension ref="A1:C45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B3" sqref="B3:B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6929,8 +6929,8 @@
   </sheetPr>
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>